<commit_message>
Skille kjørende fra trafikantgruppe G
</commit_message>
<xml_diff>
--- a/kostraleveranse2020/Kostra 05 - Fylkesveg aksellast u 10t.xlsx
+++ b/kostraleveranse2020/Kostra 05 - Fylkesveg aksellast u 10t.xlsx
@@ -450,7 +450,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="n">
-        <v>378997.4770000002</v>
+        <v>375523</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="n">
-        <v>379790.181</v>
+        <v>379790</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="n">
-        <v>587585.7079999999</v>
+        <v>586656</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>30</v>
       </c>
       <c r="B5" t="n">
-        <v>798497.2299999994</v>
+        <v>792631</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>34</v>
       </c>
       <c r="B6" t="n">
-        <v>1646721.929</v>
+        <v>1643290</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>38</v>
       </c>
       <c r="B7" t="n">
-        <v>100568.596</v>
+        <v>99643</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>42</v>
       </c>
       <c r="B8" t="n">
-        <v>533212.6370000005</v>
+        <v>532069</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>46</v>
       </c>
       <c r="B9" t="n">
-        <v>862815.7819999993</v>
+        <v>859737</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>50</v>
       </c>
       <c r="B10" t="n">
-        <v>1257624.293999999</v>
+        <v>1255210</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>54</v>
       </c>
       <c r="B11" t="n">
-        <v>1004287.877999999</v>
+        <v>1001920</v>
       </c>
     </row>
   </sheetData>

</xml_diff>